<commit_message>
create test file for cutadapt
</commit_message>
<xml_diff>
--- a/gene_expression/bioinformatics_pipeline/readcounts_allsteps_checkagainstMS.xlsx
+++ b/gene_expression/bioinformatics_pipeline/readcounts_allsteps_checkagainstMS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miamiedu-my.sharepoint.com/personal/and128_miami_edu/Documents/GitHub/Ch2_temperaturevariability2023/gene_expression/bioinformatics_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD0676A9-DCF1-D347-8A65-AC01AF31CE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{BD0676A9-DCF1-D347-8A65-AC01AF31CE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54FE7072-E1C7-1341-BF1C-B0964F795716}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="16300" windowHeight="16240" xr2:uid="{E30E7334-B642-5E4F-95D2-E511D28C5524}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="23000" windowHeight="16240" xr2:uid="{E30E7334-B642-5E4F-95D2-E511D28C5524}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1335,7 +1335,7 @@
   <dimension ref="A1:G97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A2" sqref="A2:B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1375,7 +1375,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>633051</v>
+        <v>11893867</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>99</v>
@@ -1398,7 +1398,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>845271</v>
+        <v>13209851</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>100</v>
@@ -1421,7 +1421,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>842539</v>
+        <v>13340389</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>101</v>
@@ -1444,7 +1444,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>762393</v>
+        <v>11816133</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>102</v>
@@ -1467,7 +1467,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>884256</v>
+        <v>13786013</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>103</v>
@@ -1490,7 +1490,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>750288</v>
+        <v>11690763</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>104</v>
@@ -1513,7 +1513,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>816086</v>
+        <v>12892034</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>105</v>
@@ -1536,7 +1536,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>951133</v>
+        <v>15041032</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>106</v>
@@ -1559,7 +1559,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>723219</v>
+        <v>11570068</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>107</v>
@@ -1582,7 +1582,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>866061</v>
+        <v>13899610</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>108</v>
@@ -1605,7 +1605,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>891353</v>
+        <v>14013158</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>109</v>
@@ -1628,7 +1628,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>841393</v>
+        <v>13173395</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>110</v>
@@ -1651,7 +1651,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>928217</v>
+        <v>14424718</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>111</v>
@@ -1674,7 +1674,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>756040</v>
+        <v>11795849</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>112</v>
@@ -1697,7 +1697,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1">
-        <v>1014256</v>
+        <v>16734417</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>113</v>
@@ -1720,7 +1720,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1">
-        <v>804231</v>
+        <v>13126670</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>114</v>
@@ -1743,7 +1743,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1">
-        <v>815254</v>
+        <v>13417235</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>115</v>
@@ -1766,7 +1766,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1">
-        <v>890269</v>
+        <v>13968542</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>116</v>
@@ -1789,7 +1789,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1">
-        <v>867868</v>
+        <v>13687891</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>117</v>
@@ -1812,7 +1812,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1">
-        <v>522684</v>
+        <v>8880017</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>118</v>
@@ -1835,7 +1835,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>758525</v>
+        <v>12205253</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>119</v>
@@ -1858,7 +1858,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1">
-        <v>329853</v>
+        <v>6299928</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>120</v>
@@ -1881,7 +1881,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1">
-        <v>611475</v>
+        <v>10027271</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>121</v>
@@ -1904,7 +1904,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1">
-        <v>832281</v>
+        <v>12982523</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>122</v>
@@ -1927,7 +1927,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1">
-        <v>575208</v>
+        <v>8999379</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>123</v>
@@ -1950,7 +1950,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1">
-        <v>554657</v>
+        <v>8925185</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>124</v>
@@ -1973,7 +1973,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="1">
-        <v>687954</v>
+        <v>10765315</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>125</v>
@@ -1996,7 +1996,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="1">
-        <v>385259</v>
+        <v>6642725</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>126</v>
@@ -2019,7 +2019,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="1">
-        <v>611518</v>
+        <v>9667701</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>127</v>
@@ -2042,7 +2042,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="1">
-        <v>812797</v>
+        <v>12461234</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>128</v>
@@ -2065,7 +2065,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="1">
-        <v>741349</v>
+        <v>11546185</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>129</v>
@@ -2088,7 +2088,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="1">
-        <v>747466</v>
+        <v>11893894</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>130</v>
@@ -2111,7 +2111,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="1">
-        <v>596354</v>
+        <v>9525611</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>131</v>
@@ -2134,7 +2134,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="1">
-        <v>692197</v>
+        <v>10786783</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>132</v>
@@ -2157,7 +2157,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="1">
-        <v>755893</v>
+        <v>11865741</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>133</v>
@@ -2180,7 +2180,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="1">
-        <v>399376</v>
+        <v>6537998</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>134</v>
@@ -2203,7 +2203,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="1">
-        <v>845817</v>
+        <v>13224558</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>135</v>
@@ -2226,7 +2226,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="1">
-        <v>865250</v>
+        <v>13680610</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>136</v>
@@ -2249,7 +2249,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="1">
-        <v>931136</v>
+        <v>14877314</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>137</v>
@@ -2272,7 +2272,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="1">
-        <v>483740</v>
+        <v>7959769</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>138</v>
@@ -2295,7 +2295,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="1">
-        <v>506216</v>
+        <v>8075522</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>139</v>
@@ -2318,7 +2318,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="1">
-        <v>844605</v>
+        <v>13426280</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>140</v>
@@ -2341,7 +2341,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="1">
-        <v>654939</v>
+        <v>10239279</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>141</v>
@@ -2364,7 +2364,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="1">
-        <v>1031194</v>
+        <v>16437956</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>142</v>
@@ -2387,7 +2387,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="1">
-        <v>876595</v>
+        <v>13820239</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>143</v>
@@ -2410,7 +2410,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="1">
-        <v>502327</v>
+        <v>8023742</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>144</v>
@@ -2433,7 +2433,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="1">
-        <v>537850</v>
+        <v>8962152</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>145</v>
@@ -2456,7 +2456,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="1">
-        <v>627638</v>
+        <v>9775896</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>146</v>
@@ -2479,7 +2479,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="1">
-        <v>706993</v>
+        <v>12246859</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>147</v>
@@ -2502,7 +2502,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="1">
-        <v>145832</v>
+        <v>2614591</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>148</v>
@@ -2525,7 +2525,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="1">
-        <v>548588</v>
+        <v>9496745</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>149</v>
@@ -2548,7 +2548,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="1">
-        <v>645799</v>
+        <v>10885135</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>150</v>
@@ -2571,7 +2571,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="1">
-        <v>21977</v>
+        <v>392451</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>151</v>
@@ -2594,7 +2594,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="1">
-        <v>207786</v>
+        <v>3652472</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>152</v>
@@ -2617,7 +2617,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="1">
-        <v>220062</v>
+        <v>3868556</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>153</v>
@@ -2640,7 +2640,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="1">
-        <v>964759</v>
+        <v>16822781</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>154</v>
@@ -2663,7 +2663,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="1">
-        <v>1100963</v>
+        <v>19393115</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>155</v>
@@ -2686,7 +2686,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="1">
-        <v>894746</v>
+        <v>15668221</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>156</v>
@@ -2709,7 +2709,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="1">
-        <v>868817</v>
+        <v>15100209</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>157</v>
@@ -2732,7 +2732,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="1">
-        <v>1057525</v>
+        <v>18575961</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>158</v>
@@ -2755,7 +2755,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="1">
-        <v>683159</v>
+        <v>11725284</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>159</v>
@@ -2778,7 +2778,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="1">
-        <v>171179</v>
+        <v>3000014</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>160</v>
@@ -2801,7 +2801,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="1">
-        <v>524965</v>
+        <v>9165183</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>161</v>
@@ -2824,7 +2824,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="1">
-        <v>95050</v>
+        <v>1745492</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>162</v>
@@ -2847,7 +2847,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="1">
-        <v>679315</v>
+        <v>11664169</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>163</v>
@@ -2870,7 +2870,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="1">
-        <v>611197</v>
+        <v>10468927</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>164</v>
@@ -2893,7 +2893,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="1">
-        <v>1167756</v>
+        <v>21234558</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>165</v>
@@ -2916,7 +2916,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="1">
-        <v>153502</v>
+        <v>2770431</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>166</v>
@@ -2939,7 +2939,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="1">
-        <v>68328</v>
+        <v>1239658</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>167</v>
@@ -2962,7 +2962,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="1">
-        <v>57501</v>
+        <v>1050762</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>168</v>
@@ -2985,7 +2985,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="1">
-        <v>35649</v>
+        <v>663230</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>169</v>
@@ -3008,7 +3008,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="1">
-        <v>239468</v>
+        <v>4273792</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>170</v>
@@ -3031,7 +3031,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="1">
-        <v>86376</v>
+        <v>1509835</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>171</v>
@@ -3054,7 +3054,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="1">
-        <v>862495</v>
+        <v>15036329</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>172</v>
@@ -3077,7 +3077,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="1">
-        <v>959495</v>
+        <v>16893955</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>173</v>
@@ -3100,7 +3100,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="1">
-        <v>216724</v>
+        <v>3822709</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>174</v>
@@ -3123,7 +3123,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="1">
-        <v>558591</v>
+        <v>9536367</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>175</v>
@@ -3146,7 +3146,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="1">
-        <v>208720</v>
+        <v>3754659</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>176</v>
@@ -3169,7 +3169,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="1">
-        <v>578632</v>
+        <v>10000767</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>177</v>
@@ -3192,7 +3192,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="1">
-        <v>632543</v>
+        <v>10965339</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>178</v>
@@ -3215,7 +3215,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="1">
-        <v>596784</v>
+        <v>10197898</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>179</v>
@@ -3238,7 +3238,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="1">
-        <v>186088</v>
+        <v>3268809</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>180</v>
@@ -3261,7 +3261,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="1">
-        <v>563791</v>
+        <v>9722436</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>181</v>
@@ -3284,7 +3284,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="1">
-        <v>965253</v>
+        <v>16685316</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>182</v>
@@ -3307,7 +3307,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="1">
-        <v>928970</v>
+        <v>16128393</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>183</v>
@@ -3330,7 +3330,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="1">
-        <v>651911</v>
+        <v>11145711</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>184</v>
@@ -3353,7 +3353,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="1">
-        <v>25542</v>
+        <v>473700</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>185</v>
@@ -3376,7 +3376,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="1">
-        <v>628025</v>
+        <v>10813124</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>186</v>
@@ -3399,7 +3399,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="1">
-        <v>1165055</v>
+        <v>20639733</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>187</v>
@@ -3422,7 +3422,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="1">
-        <v>167227</v>
+        <v>2952368</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>188</v>
@@ -3445,7 +3445,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="1">
-        <v>1152348</v>
+        <v>20201567</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>189</v>
@@ -3468,7 +3468,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="1">
-        <v>1350264</v>
+        <v>23415093</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>190</v>
@@ -3491,7 +3491,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="1">
-        <v>1331198</v>
+        <v>23864440</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>191</v>
@@ -3514,7 +3514,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="1">
-        <v>28189</v>
+        <v>506825</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>192</v>
@@ -3537,7 +3537,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="1">
-        <v>198319</v>
+        <v>3532817</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>193</v>
@@ -3560,7 +3560,7 @@
         <v>95</v>
       </c>
       <c r="B97" s="1">
-        <v>877106</v>
+        <v>15270107</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>194</v>

</xml_diff>